<commit_message>
Atualização da lista de requisitos pós brainstorm
</commit_message>
<xml_diff>
--- a/PastaDocsRequisitos/2SIR-ListaPesquisa.xlsx
+++ b/PastaDocsRequisitos/2SIR-ListaPesquisa.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20383"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\logonpflocal\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felip\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{493AFFA2-418E-44CF-8EEC-2822F5EB7756}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4901AB55-976A-496C-8A00-78FE68306E91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6825" xr2:uid="{0891ED88-779E-4904-AB47-DA324D9A5ACC}"/>
+    <workbookView xWindow="3384" yWindow="3384" windowWidth="17280" windowHeight="8964" xr2:uid="{0891ED88-779E-4904-AB47-DA324D9A5ACC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Requisitos do sistema de gestão de estacionamento</t>
   </si>
@@ -109,14 +109,35 @@
   </si>
   <si>
     <t>.Cadastramento e tipificaçao de vaga</t>
+  </si>
+  <si>
+    <t>.Integração com o sistema da polícia sobre carros roubados</t>
+  </si>
+  <si>
+    <t>(pos-brainstorm)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -144,8 +165,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -164,7 +187,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -460,153 +483,162 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27CD8592-6EB6-4B54-8F7E-C6467C02028C}">
-  <dimension ref="A1:A29"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>27</v>
       </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G31" t="s">
+        <v>29</v>
+      </c>
+      <c r="J31" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -614,6 +646,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100A647E37EC11C8246B76D75C67DE7970E" ma:contentTypeVersion="10" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="17c6482bd86435de73722152b5b3d04c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a6194295-1792-4b63-878c-b29c2ff82726" xmlns:ns3="49c50ba2-eaf4-4058-b769-73a32109933c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c1f1ade926c4aee093040732ea80b3eb" ns2:_="" ns3:_="">
     <xsd:import namespace="a6194295-1792-4b63-878c-b29c2ff82726"/>
@@ -816,29 +863,38 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3CC2AEF2-026D-4D4C-9292-73B356E922D7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{35A2AA33-B870-497C-A6E7-B31A9EADA4D8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{487F935D-3D72-4A02-AD9E-5F77F9D44DFF}"/>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{35A2AA33-B870-497C-A6E7-B31A9EADA4D8}"/>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3CC2AEF2-026D-4D4C-9292-73B356E922D7}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{487F935D-3D72-4A02-AD9E-5F77F9D44DFF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="a6194295-1792-4b63-878c-b29c2ff82726"/>
+    <ds:schemaRef ds:uri="49c50ba2-eaf4-4058-b769-73a32109933c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>